<commit_message>
added unit test for futures read conventions from XLS file get_convention clean-up instruments tenor formatter for plotting
</commit_message>
<xml_diff>
--- a/engine_usd_gbp.xlsx
+++ b/engine_usd_gbp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="13920" windowHeight="4950" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="13920" windowHeight="4950"/>
   </bookViews>
   <sheets>
     <sheet name="Instrument Properties" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2281" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2341" uniqueCount="77">
   <si>
     <t>3M</t>
   </si>
@@ -706,9 +706,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L235"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H170" sqref="H170"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -6086,24 +6086,22 @@
         <v>61</v>
       </c>
       <c r="D134" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E134" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F134" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G134" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H134" s="10" t="str">
-        <f>D134</f>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I134" s="10" t="str">
-        <f>H134</f>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H134" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I134" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J134" s="10" t="s">
         <v>16</v>
@@ -6127,24 +6125,22 @@
         <v>61</v>
       </c>
       <c r="D135" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F135" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G135" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H135" s="10" t="str">
-        <f t="shared" ref="H135:H163" si="11">D135</f>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I135" s="10" t="str">
-        <f t="shared" ref="I135:I163" si="12">H135</f>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H135" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I135" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J135" s="10" t="s">
         <v>16</v>
@@ -6168,24 +6164,22 @@
         <v>61</v>
       </c>
       <c r="D136" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E136" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F136" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G136" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H136" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I136" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H136" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I136" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J136" s="10" t="s">
         <v>16</v>
@@ -6209,24 +6203,22 @@
         <v>61</v>
       </c>
       <c r="D137" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E137" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F137" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G137" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H137" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I137" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H137" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I137" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J137" s="10" t="s">
         <v>16</v>
@@ -6250,24 +6242,22 @@
         <v>61</v>
       </c>
       <c r="D138" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E138" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F138" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G138" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H138" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I138" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H138" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I138" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J138" s="10" t="s">
         <v>16</v>
@@ -6291,24 +6281,22 @@
         <v>61</v>
       </c>
       <c r="D139" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E139" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F139" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G139" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H139" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I139" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H139" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I139" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J139" s="10" t="s">
         <v>16</v>
@@ -6332,24 +6320,22 @@
         <v>61</v>
       </c>
       <c r="D140" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E140" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F140" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G140" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H140" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I140" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H140" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I140" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J140" s="10" t="s">
         <v>16</v>
@@ -6373,24 +6359,22 @@
         <v>61</v>
       </c>
       <c r="D141" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E141" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F141" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G141" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H141" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I141" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H141" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I141" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J141" s="10" t="s">
         <v>16</v>
@@ -6414,24 +6398,22 @@
         <v>61</v>
       </c>
       <c r="D142" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E142" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F142" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G142" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H142" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I142" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H142" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I142" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J142" s="10" t="s">
         <v>16</v>
@@ -6455,24 +6437,22 @@
         <v>61</v>
       </c>
       <c r="D143" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E143" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F143" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G143" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H143" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I143" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H143" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I143" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J143" s="10" t="s">
         <v>16</v>
@@ -6496,24 +6476,22 @@
         <v>61</v>
       </c>
       <c r="D144" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E144" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F144" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G144" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H144" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I144" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H144" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I144" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J144" s="10" t="s">
         <v>16</v>
@@ -6537,24 +6515,22 @@
         <v>61</v>
       </c>
       <c r="D145" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E145" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F145" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G145" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H145" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I145" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H145" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I145" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J145" s="10" t="s">
         <v>16</v>
@@ -6578,24 +6554,22 @@
         <v>61</v>
       </c>
       <c r="D146" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E146" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F146" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G146" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H146" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I146" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H146" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I146" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J146" s="10" t="s">
         <v>16</v>
@@ -6619,24 +6593,22 @@
         <v>61</v>
       </c>
       <c r="D147" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E147" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F147" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G147" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H147" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I147" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H147" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I147" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J147" s="10" t="s">
         <v>16</v>
@@ -6660,24 +6632,22 @@
         <v>61</v>
       </c>
       <c r="D148" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E148" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F148" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G148" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H148" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I148" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H148" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I148" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J148" s="10" t="s">
         <v>16</v>
@@ -6701,24 +6671,22 @@
         <v>61</v>
       </c>
       <c r="D149" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E149" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F149" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G149" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H149" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I149" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H149" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I149" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J149" s="10" t="s">
         <v>16</v>
@@ -6742,24 +6710,22 @@
         <v>61</v>
       </c>
       <c r="D150" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E150" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F150" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G150" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H150" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I150" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H150" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I150" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J150" s="10" t="s">
         <v>16</v>
@@ -6783,24 +6749,22 @@
         <v>61</v>
       </c>
       <c r="D151" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E151" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F151" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G151" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H151" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I151" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H151" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I151" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J151" s="10" t="s">
         <v>16</v>
@@ -6824,24 +6788,22 @@
         <v>61</v>
       </c>
       <c r="D152" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E152" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F152" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G152" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H152" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I152" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H152" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I152" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J152" s="10" t="s">
         <v>16</v>
@@ -6865,24 +6827,22 @@
         <v>61</v>
       </c>
       <c r="D153" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E153" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F153" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G153" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H153" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I153" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H153" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I153" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J153" s="10" t="s">
         <v>16</v>
@@ -6906,24 +6866,22 @@
         <v>61</v>
       </c>
       <c r="D154" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E154" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F154" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G154" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H154" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I154" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H154" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I154" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J154" s="10" t="s">
         <v>16</v>
@@ -6947,24 +6905,22 @@
         <v>61</v>
       </c>
       <c r="D155" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E155" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F155" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G155" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H155" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I155" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H155" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I155" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J155" s="10" t="s">
         <v>16</v>
@@ -6988,24 +6944,22 @@
         <v>61</v>
       </c>
       <c r="D156" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E156" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F156" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G156" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H156" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I156" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H156" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I156" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J156" s="10" t="s">
         <v>16</v>
@@ -7029,24 +6983,22 @@
         <v>61</v>
       </c>
       <c r="D157" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E157" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F157" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G157" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H157" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I157" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H157" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I157" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J157" s="10" t="s">
         <v>16</v>
@@ -7070,24 +7022,22 @@
         <v>61</v>
       </c>
       <c r="D158" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E158" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F158" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G158" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H158" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I158" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H158" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I158" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J158" s="10" t="s">
         <v>16</v>
@@ -7111,24 +7061,22 @@
         <v>61</v>
       </c>
       <c r="D159" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E159" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F159" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G159" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H159" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I159" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H159" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I159" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J159" s="10" t="s">
         <v>16</v>
@@ -7152,24 +7100,22 @@
         <v>61</v>
       </c>
       <c r="D160" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E160" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F160" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G160" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H160" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I160" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H160" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I160" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J160" s="10" t="s">
         <v>16</v>
@@ -7193,24 +7139,22 @@
         <v>61</v>
       </c>
       <c r="D161" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E161" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F161" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G161" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H161" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I161" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H161" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I161" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J161" s="10" t="s">
         <v>16</v>
@@ -7234,24 +7178,22 @@
         <v>61</v>
       </c>
       <c r="D162" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E162" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F162" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G162" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H162" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I162" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H162" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I162" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J162" s="10" t="s">
         <v>16</v>
@@ -7275,24 +7217,22 @@
         <v>61</v>
       </c>
       <c r="D163" s="10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E163" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F163" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G163" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H163" s="10" t="str">
-        <f t="shared" si="11"/>
-        <v>USDLIBOR3M</v>
-      </c>
-      <c r="I163" s="10" t="str">
-        <f t="shared" si="12"/>
-        <v>USDLIBOR3M</v>
+        <v>66</v>
+      </c>
+      <c r="H163" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I163" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="J163" s="10" t="s">
         <v>16</v>
@@ -7329,7 +7269,7 @@
         <v>51</v>
       </c>
       <c r="H164" s="11" t="str">
-        <f t="shared" ref="H164:H178" si="13">B164</f>
+        <f t="shared" ref="H164:H178" si="11">B164</f>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I164" s="11" t="s">
@@ -7357,7 +7297,7 @@
         <v>2</v>
       </c>
       <c r="D165" s="11" t="str">
-        <f t="shared" ref="D165:D202" si="14">B165</f>
+        <f t="shared" ref="D165:D202" si="12">B165</f>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E165" s="11" t="s">
@@ -7370,7 +7310,7 @@
         <v>51</v>
       </c>
       <c r="H165" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I165" s="11" t="s">
@@ -7388,7 +7328,7 @@
     </row>
     <row r="166" spans="1:12">
       <c r="A166" s="11" t="str">
-        <f t="shared" ref="A166:A177" si="15">CONCATENATE(B165,"__Future__",J166,"_",K166)</f>
+        <f t="shared" ref="A166:A177" si="13">CONCATENATE(B165,"__Future__",J166,"_",K166)</f>
         <v>GBPLIBOR3M__Future__2F_3M</v>
       </c>
       <c r="B166" s="11" t="s">
@@ -7398,7 +7338,7 @@
         <v>2</v>
       </c>
       <c r="D166" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E166" s="11" t="s">
@@ -7411,7 +7351,7 @@
         <v>51</v>
       </c>
       <c r="H166" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I166" s="11" t="s">
@@ -7429,7 +7369,7 @@
     </row>
     <row r="167" spans="1:12">
       <c r="A167" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>GBPLIBOR3M__Future__3F_3M</v>
       </c>
       <c r="B167" s="11" t="s">
@@ -7439,7 +7379,7 @@
         <v>2</v>
       </c>
       <c r="D167" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E167" s="11" t="s">
@@ -7452,7 +7392,7 @@
         <v>51</v>
       </c>
       <c r="H167" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I167" s="11" t="s">
@@ -7470,7 +7410,7 @@
     </row>
     <row r="168" spans="1:12">
       <c r="A168" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>GBPLIBOR3M__Future__4F_3M</v>
       </c>
       <c r="B168" s="11" t="s">
@@ -7480,7 +7420,7 @@
         <v>2</v>
       </c>
       <c r="D168" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E168" s="11" t="s">
@@ -7493,7 +7433,7 @@
         <v>51</v>
       </c>
       <c r="H168" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I168" s="11" t="s">
@@ -7511,7 +7451,7 @@
     </row>
     <row r="169" spans="1:12">
       <c r="A169" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>GBPLIBOR3M__Future__5F_3M</v>
       </c>
       <c r="B169" s="11" t="s">
@@ -7521,7 +7461,7 @@
         <v>2</v>
       </c>
       <c r="D169" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E169" s="11" t="s">
@@ -7534,7 +7474,7 @@
         <v>51</v>
       </c>
       <c r="H169" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I169" s="11" t="s">
@@ -7552,7 +7492,7 @@
     </row>
     <row r="170" spans="1:12">
       <c r="A170" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>GBPLIBOR3M__Future__6F_3M</v>
       </c>
       <c r="B170" s="11" t="s">
@@ -7562,7 +7502,7 @@
         <v>2</v>
       </c>
       <c r="D170" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E170" s="11" t="s">
@@ -7575,7 +7515,7 @@
         <v>51</v>
       </c>
       <c r="H170" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I170" s="11" t="s">
@@ -7593,7 +7533,7 @@
     </row>
     <row r="171" spans="1:12">
       <c r="A171" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>GBPLIBOR3M__Future__7F_3M</v>
       </c>
       <c r="B171" s="11" t="s">
@@ -7603,7 +7543,7 @@
         <v>2</v>
       </c>
       <c r="D171" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E171" s="11" t="s">
@@ -7616,7 +7556,7 @@
         <v>51</v>
       </c>
       <c r="H171" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I171" s="11" t="s">
@@ -7634,7 +7574,7 @@
     </row>
     <row r="172" spans="1:12">
       <c r="A172" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>GBPLIBOR3M__Future__8F_3M</v>
       </c>
       <c r="B172" s="11" t="s">
@@ -7644,7 +7584,7 @@
         <v>2</v>
       </c>
       <c r="D172" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E172" s="11" t="s">
@@ -7657,7 +7597,7 @@
         <v>51</v>
       </c>
       <c r="H172" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I172" s="11" t="s">
@@ -7675,7 +7615,7 @@
     </row>
     <row r="173" spans="1:12">
       <c r="A173" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>GBPLIBOR3M__Future__9F_3M</v>
       </c>
       <c r="B173" s="11" t="s">
@@ -7685,7 +7625,7 @@
         <v>2</v>
       </c>
       <c r="D173" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E173" s="11" t="s">
@@ -7698,7 +7638,7 @@
         <v>51</v>
       </c>
       <c r="H173" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I173" s="11" t="s">
@@ -7716,7 +7656,7 @@
     </row>
     <row r="174" spans="1:12">
       <c r="A174" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>GBPLIBOR3M__Future__10F_3M</v>
       </c>
       <c r="B174" s="11" t="s">
@@ -7726,7 +7666,7 @@
         <v>2</v>
       </c>
       <c r="D174" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E174" s="11" t="s">
@@ -7739,7 +7679,7 @@
         <v>51</v>
       </c>
       <c r="H174" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I174" s="11" t="s">
@@ -7757,7 +7697,7 @@
     </row>
     <row r="175" spans="1:12">
       <c r="A175" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>GBPLIBOR3M__Future__11F_3M</v>
       </c>
       <c r="B175" s="11" t="s">
@@ -7767,7 +7707,7 @@
         <v>2</v>
       </c>
       <c r="D175" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E175" s="11" t="s">
@@ -7780,7 +7720,7 @@
         <v>51</v>
       </c>
       <c r="H175" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I175" s="11" t="s">
@@ -7798,7 +7738,7 @@
     </row>
     <row r="176" spans="1:12">
       <c r="A176" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>GBPLIBOR3M__Future__12F_3M</v>
       </c>
       <c r="B176" s="11" t="s">
@@ -7808,7 +7748,7 @@
         <v>2</v>
       </c>
       <c r="D176" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E176" s="11" t="s">
@@ -7821,7 +7761,7 @@
         <v>51</v>
       </c>
       <c r="H176" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I176" s="11" t="s">
@@ -7839,7 +7779,7 @@
     </row>
     <row r="177" spans="1:12">
       <c r="A177" s="11" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>GBPLIBOR3M__Future__13F_3M</v>
       </c>
       <c r="B177" s="11" t="s">
@@ -7849,7 +7789,7 @@
         <v>2</v>
       </c>
       <c r="D177" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E177" s="11" t="s">
@@ -7862,7 +7802,7 @@
         <v>51</v>
       </c>
       <c r="H177" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I177" s="11" t="s">
@@ -7890,7 +7830,7 @@
         <v>17</v>
       </c>
       <c r="D178" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E178" s="11" t="s">
@@ -7903,7 +7843,7 @@
         <v>51</v>
       </c>
       <c r="H178" s="11" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I178" s="11" t="str">
@@ -7922,7 +7862,7 @@
     </row>
     <row r="179" spans="1:12">
       <c r="A179" s="11" t="str">
-        <f t="shared" ref="A179:A202" si="16">CONCATENATE(B179,"__Swap__",K179)</f>
+        <f t="shared" ref="A179:A202" si="14">CONCATENATE(B179,"__Swap__",K179)</f>
         <v>GBPLIBOR3M__Swap__5Y</v>
       </c>
       <c r="B179" s="11" t="s">
@@ -7932,7 +7872,7 @@
         <v>17</v>
       </c>
       <c r="D179" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E179" s="11" t="s">
@@ -7945,11 +7885,11 @@
         <v>51</v>
       </c>
       <c r="H179" s="11" t="str">
-        <f t="shared" ref="H179:H202" si="17">B179</f>
+        <f t="shared" ref="H179:H202" si="15">B179</f>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I179" s="11" t="str">
-        <f t="shared" ref="I179:I202" si="18">B179</f>
+        <f t="shared" ref="I179:I202" si="16">B179</f>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J179" s="11" t="s">
@@ -7964,7 +7904,7 @@
     </row>
     <row r="180" spans="1:12">
       <c r="A180" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__6Y</v>
       </c>
       <c r="B180" s="11" t="s">
@@ -7974,7 +7914,7 @@
         <v>17</v>
       </c>
       <c r="D180" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E180" s="11" t="s">
@@ -7987,11 +7927,11 @@
         <v>51</v>
       </c>
       <c r="H180" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I180" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J180" s="11" t="s">
@@ -8006,7 +7946,7 @@
     </row>
     <row r="181" spans="1:12">
       <c r="A181" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__7Y</v>
       </c>
       <c r="B181" s="11" t="s">
@@ -8016,7 +7956,7 @@
         <v>17</v>
       </c>
       <c r="D181" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E181" s="11" t="s">
@@ -8029,11 +7969,11 @@
         <v>51</v>
       </c>
       <c r="H181" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I181" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J181" s="11" t="s">
@@ -8048,7 +7988,7 @@
     </row>
     <row r="182" spans="1:12">
       <c r="A182" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__8Y</v>
       </c>
       <c r="B182" s="11" t="s">
@@ -8058,7 +7998,7 @@
         <v>17</v>
       </c>
       <c r="D182" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E182" s="11" t="s">
@@ -8071,11 +8011,11 @@
         <v>51</v>
       </c>
       <c r="H182" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I182" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J182" s="11" t="s">
@@ -8090,7 +8030,7 @@
     </row>
     <row r="183" spans="1:12">
       <c r="A183" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__9Y</v>
       </c>
       <c r="B183" s="11" t="s">
@@ -8100,7 +8040,7 @@
         <v>17</v>
       </c>
       <c r="D183" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E183" s="11" t="s">
@@ -8113,11 +8053,11 @@
         <v>51</v>
       </c>
       <c r="H183" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I183" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J183" s="11" t="s">
@@ -8132,7 +8072,7 @@
     </row>
     <row r="184" spans="1:12">
       <c r="A184" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__10Y</v>
       </c>
       <c r="B184" s="11" t="s">
@@ -8142,7 +8082,7 @@
         <v>17</v>
       </c>
       <c r="D184" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E184" s="11" t="s">
@@ -8155,11 +8095,11 @@
         <v>51</v>
       </c>
       <c r="H184" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I184" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J184" s="11" t="s">
@@ -8174,7 +8114,7 @@
     </row>
     <row r="185" spans="1:12">
       <c r="A185" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__11Y</v>
       </c>
       <c r="B185" s="11" t="s">
@@ -8184,7 +8124,7 @@
         <v>17</v>
       </c>
       <c r="D185" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E185" s="11" t="s">
@@ -8197,11 +8137,11 @@
         <v>51</v>
       </c>
       <c r="H185" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I185" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J185" s="11" t="s">
@@ -8216,7 +8156,7 @@
     </row>
     <row r="186" spans="1:12">
       <c r="A186" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__12Y</v>
       </c>
       <c r="B186" s="11" t="s">
@@ -8226,7 +8166,7 @@
         <v>17</v>
       </c>
       <c r="D186" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E186" s="11" t="s">
@@ -8239,11 +8179,11 @@
         <v>51</v>
       </c>
       <c r="H186" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I186" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J186" s="11" t="s">
@@ -8258,7 +8198,7 @@
     </row>
     <row r="187" spans="1:12">
       <c r="A187" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__13Y</v>
       </c>
       <c r="B187" s="11" t="s">
@@ -8268,7 +8208,7 @@
         <v>17</v>
       </c>
       <c r="D187" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E187" s="11" t="s">
@@ -8281,11 +8221,11 @@
         <v>51</v>
       </c>
       <c r="H187" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I187" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J187" s="11" t="s">
@@ -8300,7 +8240,7 @@
     </row>
     <row r="188" spans="1:12">
       <c r="A188" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__14Y</v>
       </c>
       <c r="B188" s="11" t="s">
@@ -8310,7 +8250,7 @@
         <v>17</v>
       </c>
       <c r="D188" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E188" s="11" t="s">
@@ -8323,11 +8263,11 @@
         <v>51</v>
       </c>
       <c r="H188" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I188" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J188" s="11" t="s">
@@ -8342,7 +8282,7 @@
     </row>
     <row r="189" spans="1:12">
       <c r="A189" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__15Y</v>
       </c>
       <c r="B189" s="11" t="s">
@@ -8352,7 +8292,7 @@
         <v>17</v>
       </c>
       <c r="D189" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E189" s="11" t="s">
@@ -8365,11 +8305,11 @@
         <v>51</v>
       </c>
       <c r="H189" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I189" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J189" s="11" t="s">
@@ -8384,7 +8324,7 @@
     </row>
     <row r="190" spans="1:12">
       <c r="A190" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__16Y</v>
       </c>
       <c r="B190" s="11" t="s">
@@ -8394,7 +8334,7 @@
         <v>17</v>
       </c>
       <c r="D190" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E190" s="11" t="s">
@@ -8407,11 +8347,11 @@
         <v>51</v>
       </c>
       <c r="H190" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I190" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J190" s="11" t="s">
@@ -8426,7 +8366,7 @@
     </row>
     <row r="191" spans="1:12">
       <c r="A191" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__17Y</v>
       </c>
       <c r="B191" s="11" t="s">
@@ -8436,7 +8376,7 @@
         <v>17</v>
       </c>
       <c r="D191" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E191" s="11" t="s">
@@ -8449,11 +8389,11 @@
         <v>51</v>
       </c>
       <c r="H191" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I191" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J191" s="11" t="s">
@@ -8468,7 +8408,7 @@
     </row>
     <row r="192" spans="1:12">
       <c r="A192" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__18Y</v>
       </c>
       <c r="B192" s="11" t="s">
@@ -8478,7 +8418,7 @@
         <v>17</v>
       </c>
       <c r="D192" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E192" s="11" t="s">
@@ -8491,11 +8431,11 @@
         <v>51</v>
       </c>
       <c r="H192" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I192" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J192" s="11" t="s">
@@ -8510,7 +8450,7 @@
     </row>
     <row r="193" spans="1:12">
       <c r="A193" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__19Y</v>
       </c>
       <c r="B193" s="11" t="s">
@@ -8520,7 +8460,7 @@
         <v>17</v>
       </c>
       <c r="D193" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E193" s="11" t="s">
@@ -8533,11 +8473,11 @@
         <v>51</v>
       </c>
       <c r="H193" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I193" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J193" s="11" t="s">
@@ -8552,7 +8492,7 @@
     </row>
     <row r="194" spans="1:12">
       <c r="A194" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__20Y</v>
       </c>
       <c r="B194" s="11" t="s">
@@ -8562,7 +8502,7 @@
         <v>17</v>
       </c>
       <c r="D194" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E194" s="11" t="s">
@@ -8575,11 +8515,11 @@
         <v>51</v>
       </c>
       <c r="H194" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I194" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J194" s="11" t="s">
@@ -8594,7 +8534,7 @@
     </row>
     <row r="195" spans="1:12">
       <c r="A195" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__25Y</v>
       </c>
       <c r="B195" s="11" t="s">
@@ -8604,7 +8544,7 @@
         <v>17</v>
       </c>
       <c r="D195" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E195" s="11" t="s">
@@ -8617,11 +8557,11 @@
         <v>51</v>
       </c>
       <c r="H195" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I195" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J195" s="11" t="s">
@@ -8636,7 +8576,7 @@
     </row>
     <row r="196" spans="1:12">
       <c r="A196" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__30Y</v>
       </c>
       <c r="B196" s="11" t="s">
@@ -8646,7 +8586,7 @@
         <v>17</v>
       </c>
       <c r="D196" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E196" s="11" t="s">
@@ -8659,11 +8599,11 @@
         <v>51</v>
       </c>
       <c r="H196" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I196" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J196" s="11" t="s">
@@ -8678,7 +8618,7 @@
     </row>
     <row r="197" spans="1:12">
       <c r="A197" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__35Y</v>
       </c>
       <c r="B197" s="11" t="s">
@@ -8688,7 +8628,7 @@
         <v>17</v>
       </c>
       <c r="D197" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E197" s="11" t="s">
@@ -8701,11 +8641,11 @@
         <v>51</v>
       </c>
       <c r="H197" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I197" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J197" s="11" t="s">
@@ -8720,7 +8660,7 @@
     </row>
     <row r="198" spans="1:12">
       <c r="A198" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__40Y</v>
       </c>
       <c r="B198" s="11" t="s">
@@ -8730,7 +8670,7 @@
         <v>17</v>
       </c>
       <c r="D198" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E198" s="11" t="s">
@@ -8743,11 +8683,11 @@
         <v>51</v>
       </c>
       <c r="H198" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I198" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J198" s="11" t="s">
@@ -8762,7 +8702,7 @@
     </row>
     <row r="199" spans="1:12">
       <c r="A199" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__45Y</v>
       </c>
       <c r="B199" s="11" t="s">
@@ -8772,7 +8712,7 @@
         <v>17</v>
       </c>
       <c r="D199" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E199" s="11" t="s">
@@ -8785,11 +8725,11 @@
         <v>51</v>
       </c>
       <c r="H199" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I199" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J199" s="11" t="s">
@@ -8804,7 +8744,7 @@
     </row>
     <row r="200" spans="1:12">
       <c r="A200" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__50Y</v>
       </c>
       <c r="B200" s="11" t="s">
@@ -8814,7 +8754,7 @@
         <v>17</v>
       </c>
       <c r="D200" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E200" s="11" t="s">
@@ -8827,11 +8767,11 @@
         <v>51</v>
       </c>
       <c r="H200" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I200" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J200" s="11" t="s">
@@ -8846,7 +8786,7 @@
     </row>
     <row r="201" spans="1:12">
       <c r="A201" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__60Y</v>
       </c>
       <c r="B201" s="11" t="s">
@@ -8856,7 +8796,7 @@
         <v>17</v>
       </c>
       <c r="D201" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E201" s="11" t="s">
@@ -8869,11 +8809,11 @@
         <v>51</v>
       </c>
       <c r="H201" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I201" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J201" s="11" t="s">
@@ -8888,7 +8828,7 @@
     </row>
     <row r="202" spans="1:12">
       <c r="A202" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>GBPLIBOR3M__Swap__70Y</v>
       </c>
       <c r="B202" s="11" t="s">
@@ -8898,7 +8838,7 @@
         <v>17</v>
       </c>
       <c r="D202" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="E202" s="11" t="s">
@@ -8911,11 +8851,11 @@
         <v>51</v>
       </c>
       <c r="H202" s="11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="I202" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>GBPLIBOR3M</v>
       </c>
       <c r="J202" s="11" t="s">
@@ -8969,7 +8909,7 @@
     </row>
     <row r="204" spans="1:12">
       <c r="A204" s="9" t="str">
-        <f t="shared" ref="A204:A235" si="19">CONCATENATE(B204,"__TermDeposit__",K204)</f>
+        <f t="shared" ref="A204:A235" si="17">CONCATENATE(B204,"__TermDeposit__",K204)</f>
         <v>GBP-GBPSONIA__TermDeposit__1M</v>
       </c>
       <c r="B204" s="9" t="s">
@@ -9008,7 +8948,7 @@
     </row>
     <row r="205" spans="1:12">
       <c r="A205" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__2M</v>
       </c>
       <c r="B205" s="9" t="s">
@@ -9047,7 +8987,7 @@
     </row>
     <row r="206" spans="1:12">
       <c r="A206" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__3M</v>
       </c>
       <c r="B206" s="9" t="s">
@@ -9086,7 +9026,7 @@
     </row>
     <row r="207" spans="1:12">
       <c r="A207" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__6M</v>
       </c>
       <c r="B207" s="9" t="s">
@@ -9125,7 +9065,7 @@
     </row>
     <row r="208" spans="1:12">
       <c r="A208" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__1Y</v>
       </c>
       <c r="B208" s="9" t="s">
@@ -9164,7 +9104,7 @@
     </row>
     <row r="209" spans="1:12">
       <c r="A209" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__2Y</v>
       </c>
       <c r="B209" s="9" t="s">
@@ -9203,7 +9143,7 @@
     </row>
     <row r="210" spans="1:12">
       <c r="A210" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__3Y</v>
       </c>
       <c r="B210" s="9" t="s">
@@ -9242,7 +9182,7 @@
     </row>
     <row r="211" spans="1:12">
       <c r="A211" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__4Y</v>
       </c>
       <c r="B211" s="9" t="s">
@@ -9281,7 +9221,7 @@
     </row>
     <row r="212" spans="1:12">
       <c r="A212" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__5Y</v>
       </c>
       <c r="B212" s="9" t="s">
@@ -9320,7 +9260,7 @@
     </row>
     <row r="213" spans="1:12">
       <c r="A213" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__6Y</v>
       </c>
       <c r="B213" s="9" t="s">
@@ -9359,7 +9299,7 @@
     </row>
     <row r="214" spans="1:12">
       <c r="A214" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__7Y</v>
       </c>
       <c r="B214" s="9" t="s">
@@ -9398,7 +9338,7 @@
     </row>
     <row r="215" spans="1:12">
       <c r="A215" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__8Y</v>
       </c>
       <c r="B215" s="9" t="s">
@@ -9437,7 +9377,7 @@
     </row>
     <row r="216" spans="1:12">
       <c r="A216" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__9Y</v>
       </c>
       <c r="B216" s="9" t="s">
@@ -9476,7 +9416,7 @@
     </row>
     <row r="217" spans="1:12">
       <c r="A217" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__10Y</v>
       </c>
       <c r="B217" s="9" t="s">
@@ -9515,7 +9455,7 @@
     </row>
     <row r="218" spans="1:12">
       <c r="A218" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__11Y</v>
       </c>
       <c r="B218" s="9" t="s">
@@ -9554,7 +9494,7 @@
     </row>
     <row r="219" spans="1:12">
       <c r="A219" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__12Y</v>
       </c>
       <c r="B219" s="9" t="s">
@@ -9593,7 +9533,7 @@
     </row>
     <row r="220" spans="1:12">
       <c r="A220" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__13Y</v>
       </c>
       <c r="B220" s="9" t="s">
@@ -9632,7 +9572,7 @@
     </row>
     <row r="221" spans="1:12">
       <c r="A221" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__14Y</v>
       </c>
       <c r="B221" s="9" t="s">
@@ -9671,7 +9611,7 @@
     </row>
     <row r="222" spans="1:12">
       <c r="A222" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__15Y</v>
       </c>
       <c r="B222" s="9" t="s">
@@ -9710,7 +9650,7 @@
     </row>
     <row r="223" spans="1:12">
       <c r="A223" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__16Y</v>
       </c>
       <c r="B223" s="9" t="s">
@@ -9749,7 +9689,7 @@
     </row>
     <row r="224" spans="1:12">
       <c r="A224" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__17Y</v>
       </c>
       <c r="B224" s="9" t="s">
@@ -9788,7 +9728,7 @@
     </row>
     <row r="225" spans="1:12">
       <c r="A225" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__18Y</v>
       </c>
       <c r="B225" s="9" t="s">
@@ -9827,7 +9767,7 @@
     </row>
     <row r="226" spans="1:12">
       <c r="A226" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__19Y</v>
       </c>
       <c r="B226" s="9" t="s">
@@ -9866,7 +9806,7 @@
     </row>
     <row r="227" spans="1:12">
       <c r="A227" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__20Y</v>
       </c>
       <c r="B227" s="9" t="s">
@@ -9905,7 +9845,7 @@
     </row>
     <row r="228" spans="1:12">
       <c r="A228" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__25Y</v>
       </c>
       <c r="B228" s="9" t="s">
@@ -9944,7 +9884,7 @@
     </row>
     <row r="229" spans="1:12">
       <c r="A229" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__30Y</v>
       </c>
       <c r="B229" s="9" t="s">
@@ -9983,7 +9923,7 @@
     </row>
     <row r="230" spans="1:12">
       <c r="A230" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__35Y</v>
       </c>
       <c r="B230" s="9" t="s">
@@ -10022,7 +9962,7 @@
     </row>
     <row r="231" spans="1:12">
       <c r="A231" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__40Y</v>
       </c>
       <c r="B231" s="9" t="s">
@@ -10061,7 +10001,7 @@
     </row>
     <row r="232" spans="1:12">
       <c r="A232" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__45Y</v>
       </c>
       <c r="B232" s="9" t="s">
@@ -10100,7 +10040,7 @@
     </row>
     <row r="233" spans="1:12">
       <c r="A233" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__50Y</v>
       </c>
       <c r="B233" s="9" t="s">
@@ -10139,7 +10079,7 @@
     </row>
     <row r="234" spans="1:12">
       <c r="A234" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__60Y</v>
       </c>
       <c r="B234" s="9" t="s">
@@ -10178,7 +10118,7 @@
     </row>
     <row r="235" spans="1:12">
       <c r="A235" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>GBP-GBPSONIA__TermDeposit__70Y</v>
       </c>
       <c r="B235" s="9" t="s">
@@ -10261,7 +10201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>